<commit_message>
Correção de URL no frontoffice em todos os roles , melhoria testes funcionais e produtos ja mostra como guest
</commit_message>
<xml_diff>
--- a/Documentos/Template_PlanoTestes.xlsx
+++ b/Documentos/Template_PlanoTestes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JoanaPedrosa\Documents\AULAS_202021\1Semestre_PLSI\ENUNCIADO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\GestorRestauranteWEB\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E892B3-F039-431B-82FC-5515E6203A37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1DB495-E9A3-4977-8479-93A503300F83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{95683A14-184E-4B3C-BA7D-5CA753ECF9F9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{95683A14-184E-4B3C-BA7D-5CA753ECF9F9}"/>
   </bookViews>
   <sheets>
     <sheet name="PlanoTestes" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="28">
   <si>
     <t>Nome do Projeto</t>
   </si>
@@ -100,6 +100,27 @@
   </si>
   <si>
     <t>Plataformas de Sistemas de Informação       |      D + PL      |      2020/21</t>
+  </si>
+  <si>
+    <t>Carlos Eduardo Afonso Vinagre</t>
+  </si>
+  <si>
+    <t>Rui Jorge Miguel Penetra</t>
+  </si>
+  <si>
+    <t>Login no backend</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> backend/web/index.php?r=site%2Flogin</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>Signup no frontend</t>
+  </si>
+  <si>
+    <t>frontend/web/index.php?r=site%2Fsignup</t>
   </si>
 </sst>
 </file>
@@ -625,12 +646,43 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -640,73 +692,42 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1023,8 +1044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4C581CB-E1F9-4895-AECD-C1EB3A0EDA78}">
   <dimension ref="B2:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1036,54 +1057,54 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="40"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="23"/>
     </row>
     <row r="3" spans="2:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:15" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="37"/>
-      <c r="M4" s="38"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="21"/>
     </row>
     <row r="5" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:15" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="41"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="42"/>
-      <c r="K6" s="42"/>
-      <c r="L6" s="43"/>
-      <c r="M6" s="44"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="43"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="25"/>
     </row>
     <row r="7" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="3"/>
@@ -1101,56 +1122,64 @@
     </row>
     <row r="8" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="2:15" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="24"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="35"/>
     </row>
     <row r="10" spans="2:15" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="30"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="38"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C11" s="1"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="33"/>
+      <c r="C11" s="1">
+        <v>2180687</v>
+      </c>
+      <c r="D11" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="41"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C12" s="1"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="33"/>
+      <c r="C12" s="1">
+        <v>2180680</v>
+      </c>
+      <c r="D12" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="41"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C13" s="1"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="33"/>
-      <c r="O13" s="47"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="41"/>
+      <c r="O13" s="26"/>
     </row>
     <row r="16" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B16" s="6" t="s">
@@ -1161,75 +1190,75 @@
       <c r="B17" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B18" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B20" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="20"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B22" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
     </row>
     <row r="24" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B24" s="6" t="s">
@@ -1240,75 +1269,75 @@
       <c r="B25" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="21" t="s">
+      <c r="C25" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="21"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="28"/>
+      <c r="I25" s="28"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B26" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="27"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B27" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="20"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="27"/>
+      <c r="I27" s="27"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B28" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
-      <c r="I28" s="20"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="27"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B29" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="20"/>
-      <c r="I29" s="20"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B30" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B31" s="9"/>
@@ -1329,27 +1358,27 @@
       <c r="B33" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C33" s="21" t="s">
+      <c r="C33" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="21"/>
-      <c r="I33" s="21"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="28"/>
+      <c r="H33" s="28"/>
+      <c r="I33" s="28"/>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B34" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="20"/>
-      <c r="I34" s="20"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="27"/>
+      <c r="G34" s="27"/>
+      <c r="H34" s="27"/>
+      <c r="I34" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="22">
@@ -1387,7 +1416,7 @@
   <dimension ref="B2:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1399,33 +1428,33 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="27"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="45"/>
     </row>
     <row r="5" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
       <c r="I6" s="16" t="s">
         <v>16</v>
       </c>
@@ -1437,12 +1466,12 @@
       <c r="B7" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
       <c r="I7" s="11"/>
       <c r="J7" s="12"/>
     </row>
@@ -1450,12 +1479,12 @@
       <c r="B8" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
       <c r="I8" s="11"/>
       <c r="J8" s="12"/>
     </row>
@@ -1463,12 +1492,12 @@
       <c r="B9" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
       <c r="I9" s="11"/>
       <c r="J9" s="12"/>
     </row>
@@ -1476,12 +1505,12 @@
       <c r="B10" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
       <c r="I10" s="11"/>
       <c r="J10" s="12"/>
     </row>
@@ -1489,12 +1518,12 @@
       <c r="B11" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
       <c r="I11" s="13"/>
       <c r="J11" s="14"/>
     </row>
@@ -1518,44 +1547,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2388E85-4066-4F58-9827-09010DD3CF52}">
   <dimension ref="B2:L11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="9" max="9" width="13.33203125" customWidth="1"/>
+    <col min="9" max="9" width="34.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="21" x14ac:dyDescent="0.3">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="27"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="45"/>
     </row>
     <row r="5" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
       <c r="I6" s="16" t="s">
         <v>18</v>
       </c>
@@ -1567,38 +1596,48 @@
       <c r="B7" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="12"/>
+      <c r="C7" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="8" spans="2:12" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="11"/>
+      <c r="C8" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="11" t="s">
+        <v>27</v>
+      </c>
       <c r="J8" s="12"/>
     </row>
     <row r="9" spans="2:12" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
       <c r="I9" s="11"/>
       <c r="J9" s="12"/>
     </row>
@@ -1606,12 +1645,12 @@
       <c r="B10" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
       <c r="I10" s="11"/>
       <c r="J10" s="12"/>
     </row>
@@ -1619,12 +1658,12 @@
       <c r="B11" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
       <c r="I11" s="13"/>
       <c r="J11" s="14"/>
     </row>
@@ -1656,31 +1695,31 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="21" x14ac:dyDescent="0.3">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="27"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="45"/>
     </row>
     <row r="4" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
       <c r="I5" s="17" t="s">
         <v>17</v>
       </c>
@@ -1689,12 +1728,12 @@
       <c r="B6" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
       <c r="I6" s="14"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Criação do Template dos Testes
</commit_message>
<xml_diff>
--- a/Documentos/Template_PlanoTestes.xlsx
+++ b/Documentos/Template_PlanoTestes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\GestorRestauranteWEB\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1DB495-E9A3-4977-8479-93A503300F83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{597D6571-E169-43F3-A87F-D0FE34FA3D08}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{95683A14-184E-4B3C-BA7D-5CA753ECF9F9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{95683A14-184E-4B3C-BA7D-5CA753ECF9F9}"/>
   </bookViews>
   <sheets>
     <sheet name="PlanoTestes" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="56">
   <si>
     <t>Nome do Projeto</t>
   </si>
@@ -111,16 +111,100 @@
     <t>Login no backend</t>
   </si>
   <si>
-    <t xml:space="preserve"> backend/web/index.php?r=site%2Flogin</t>
-  </si>
-  <si>
-    <t>PASS</t>
-  </si>
-  <si>
-    <t>Signup no frontend</t>
-  </si>
-  <si>
-    <t>frontend/web/index.php?r=site%2Fsignup</t>
+    <t>Login no Backend</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Criar/Pesquisar Produtos</t>
+  </si>
+  <si>
+    <t>?r=categoriaproduto%2Findex</t>
+  </si>
+  <si>
+    <t>?r=site%2Flogin</t>
+  </si>
+  <si>
+    <t>Criar/Pesquisar Mesa</t>
+  </si>
+  <si>
+    <t>?r=mesa%2Findex</t>
+  </si>
+  <si>
+    <t>?r=site%2Findex</t>
+  </si>
+  <si>
+    <t>Pesquisar produto por Nome/Preço e Desativalo</t>
+  </si>
+  <si>
+    <t>Criar Novo utilizador</t>
+  </si>
+  <si>
+    <t>?r=user%2Findex</t>
+  </si>
+  <si>
+    <t>User/Perfil</t>
+  </si>
+  <si>
+    <t>PedidoProduto</t>
+  </si>
+  <si>
+    <t>Valida campos, Cria Produtos no pedido, Atualiza e Elimina</t>
+  </si>
+  <si>
+    <t>Valida Campos , Cria utilizador , Atualiza e Elimina</t>
+  </si>
+  <si>
+    <t>Valida campos, Cria pedido takeaway e restaurante Atualizando e Eliminando os mesmos</t>
+  </si>
+  <si>
+    <t>Pedido</t>
+  </si>
+  <si>
+    <t>Produto</t>
+  </si>
+  <si>
+    <t>Valida campos, Cria produto,Atualiza e Elimina</t>
+  </si>
+  <si>
+    <t>Valida campos,Cria reserva,Atualiza e Elimina</t>
+  </si>
+  <si>
+    <t>Reserva</t>
+  </si>
+  <si>
+    <t>Login no backend e verifica see ve o painel</t>
+  </si>
+  <si>
+    <t>Cria Produto</t>
+  </si>
+  <si>
+    <t>Testa se a pagina carrega</t>
+  </si>
+  <si>
+    <t>NOTA:Durante a Criação desde documento o Google Chrome Atualizou para a versao 87.0.4280.141 e o Chromedriver ainda não atualizou para a mesma versão o que faz com que os testes não sejam possiveis de testar no entanto no passado foram testados e passavam.</t>
+  </si>
+  <si>
+    <t>Validar e testar o crud do User/Perfil (excepto o read)</t>
+  </si>
+  <si>
+    <t>Validar e testar o crud do PedidoProduto (excepto o read)</t>
+  </si>
+  <si>
+    <t>Valida e testar o crud(excepto o read) dos 2 tipos de pedido existentes</t>
+  </si>
+  <si>
+    <t>Valida e testar o crud (excepto o read) dos produtos</t>
+  </si>
+  <si>
+    <t>Valida e testar o crud(excepto o read) das reservas</t>
+  </si>
+  <si>
+    <t>Criar novo Utilizador</t>
+  </si>
+  <si>
+    <t>Pesquisar Produto por nome/preço e desativalo</t>
   </si>
 </sst>
 </file>
@@ -597,7 +681,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -665,51 +749,51 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -727,6 +811,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -743,6 +830,99 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>52342</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>776695</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>133874</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{022B76FB-9C8F-422A-80FA-9B69C8EBEDB6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="693420" y="3245122"/>
+          <a:ext cx="4960075" cy="1910332"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>337819</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>76429</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagem 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4D86C50-C39F-4E0E-918C-3BC04D911623}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5814060" y="3459480"/>
+          <a:ext cx="4544059" cy="1638529"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1042,10 +1222,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4C581CB-E1F9-4895-AECD-C1EB3A0EDA78}">
-  <dimension ref="B2:O34"/>
+  <dimension ref="B2:O36"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12:I12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1057,35 +1237,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
       <c r="L2" s="22"/>
       <c r="M2" s="23"/>
     </row>
     <row r="3" spans="2:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:15" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
       <c r="L4" s="20"/>
       <c r="M4" s="21"/>
     </row>
@@ -1122,63 +1302,63 @@
     </row>
     <row r="8" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="2:15" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="33" t="s">
+      <c r="C9" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="35"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="33"/>
     </row>
     <row r="10" spans="2:15" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="36" t="s">
+      <c r="D10" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="37"/>
-      <c r="I10" s="38"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="37"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C11" s="1">
         <v>2180687</v>
       </c>
-      <c r="D11" s="39" t="s">
+      <c r="D11" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="41"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="40"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C12" s="1">
         <v>2180680</v>
       </c>
-      <c r="D12" s="39" t="s">
+      <c r="D12" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="41"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="40"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C13" s="1"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="41"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="40"/>
       <c r="O13" s="26"/>
     </row>
     <row r="16" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
@@ -1190,75 +1370,85 @@
       <c r="B17" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="28" t="s">
+      <c r="C17" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="41"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B18" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="27"/>
-      <c r="I18" s="27"/>
+      <c r="C18" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="34"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="27"/>
-      <c r="I19" s="27"/>
+      <c r="C19" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="34"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B20" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="27"/>
+      <c r="C20" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="34"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
-      <c r="I21" s="27"/>
+      <c r="C21" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="34"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B22" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="27"/>
-      <c r="I22" s="27"/>
+      <c r="C22" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="34"/>
+      <c r="I22" s="34"/>
     </row>
     <row r="24" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B24" s="6" t="s">
@@ -1269,75 +1459,85 @@
       <c r="B25" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="28" t="s">
+      <c r="C25" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="28"/>
+      <c r="D25" s="41"/>
+      <c r="E25" s="41"/>
+      <c r="F25" s="41"/>
+      <c r="G25" s="41"/>
+      <c r="H25" s="41"/>
+      <c r="I25" s="41"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B26" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="27"/>
-      <c r="I26" s="27"/>
+      <c r="C26" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="34"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="34"/>
+      <c r="H26" s="34"/>
+      <c r="I26" s="34"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B27" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="27"/>
-      <c r="I27" s="27"/>
+      <c r="C27" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="34"/>
+      <c r="I27" s="34"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B28" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="27"/>
-      <c r="I28" s="27"/>
+      <c r="C28" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28" s="34"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="34"/>
+      <c r="I28" s="34"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B29" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
+      <c r="C29" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="D29" s="34"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="34"/>
+      <c r="H29" s="34"/>
+      <c r="I29" s="34"/>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B30" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
+      <c r="C30" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" s="34"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="34"/>
+      <c r="G30" s="34"/>
+      <c r="H30" s="34"/>
+      <c r="I30" s="34"/>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B31" s="9"/>
@@ -1358,30 +1558,70 @@
       <c r="B33" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C33" s="28" t="s">
+      <c r="C33" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="D33" s="28"/>
-      <c r="E33" s="28"/>
-      <c r="F33" s="28"/>
-      <c r="G33" s="28"/>
-      <c r="H33" s="28"/>
-      <c r="I33" s="28"/>
+      <c r="D33" s="41"/>
+      <c r="E33" s="41"/>
+      <c r="F33" s="41"/>
+      <c r="G33" s="41"/>
+      <c r="H33" s="41"/>
+      <c r="I33" s="41"/>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B34" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="27"/>
-      <c r="D34" s="27"/>
-      <c r="E34" s="27"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="27"/>
-      <c r="H34" s="27"/>
-      <c r="I34" s="27"/>
+      <c r="C34" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34" s="34"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="34"/>
+      <c r="H34" s="34"/>
+      <c r="I34" s="34"/>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B35" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="D35" s="34"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="34"/>
+      <c r="G35" s="34"/>
+      <c r="H35" s="34"/>
+      <c r="I35" s="34"/>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B36" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="D36" s="34"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
+      <c r="G36" s="34"/>
+      <c r="H36" s="34"/>
+      <c r="I36" s="34"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="24">
+    <mergeCell ref="C35:I35"/>
+    <mergeCell ref="C36:I36"/>
+    <mergeCell ref="C30:I30"/>
+    <mergeCell ref="C33:I33"/>
+    <mergeCell ref="C34:I34"/>
+    <mergeCell ref="C25:I25"/>
+    <mergeCell ref="C26:I26"/>
+    <mergeCell ref="C27:I27"/>
+    <mergeCell ref="C28:I28"/>
+    <mergeCell ref="C29:I29"/>
     <mergeCell ref="B4:K4"/>
     <mergeCell ref="B2:K2"/>
     <mergeCell ref="C9:I9"/>
@@ -1396,14 +1636,6 @@
     <mergeCell ref="C20:I20"/>
     <mergeCell ref="C21:I21"/>
     <mergeCell ref="C6:K6"/>
-    <mergeCell ref="C30:I30"/>
-    <mergeCell ref="C33:I33"/>
-    <mergeCell ref="C34:I34"/>
-    <mergeCell ref="C25:I25"/>
-    <mergeCell ref="C26:I26"/>
-    <mergeCell ref="C27:I27"/>
-    <mergeCell ref="C28:I28"/>
-    <mergeCell ref="C29:I29"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1416,7 +1648,7 @@
   <dimension ref="B2:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="C10" sqref="C10:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1428,18 +1660,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
       <c r="L2" s="45"/>
     </row>
     <row r="5" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1466,66 +1698,96 @@
       <c r="B7" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="47"/>
+      <c r="C7" s="47" t="s">
+        <v>38</v>
+      </c>
       <c r="D7" s="47"/>
       <c r="E7" s="47"/>
       <c r="F7" s="47"/>
       <c r="G7" s="47"/>
       <c r="H7" s="47"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="12"/>
+      <c r="I7" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="8" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="47"/>
+      <c r="C8" s="47" t="s">
+        <v>37</v>
+      </c>
       <c r="D8" s="47"/>
       <c r="E8" s="47"/>
       <c r="F8" s="47"/>
       <c r="G8" s="47"/>
       <c r="H8" s="47"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="12"/>
+      <c r="I8" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="9" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="47"/>
+      <c r="C9" s="47" t="s">
+        <v>39</v>
+      </c>
       <c r="D9" s="47"/>
       <c r="E9" s="47"/>
       <c r="F9" s="47"/>
       <c r="G9" s="47"/>
       <c r="H9" s="47"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="12"/>
+      <c r="I9" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="10" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="47"/>
+      <c r="C10" s="47" t="s">
+        <v>42</v>
+      </c>
       <c r="D10" s="47"/>
       <c r="E10" s="47"/>
       <c r="F10" s="47"/>
       <c r="G10" s="47"/>
       <c r="H10" s="47"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="12"/>
+      <c r="I10" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="11" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="44"/>
+      <c r="C11" s="44" t="s">
+        <v>43</v>
+      </c>
       <c r="D11" s="44"/>
       <c r="E11" s="44"/>
       <c r="F11" s="44"/>
       <c r="G11" s="44"/>
       <c r="H11" s="44"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="14"/>
+      <c r="I11" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="J11" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1547,8 +1809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2388E85-4066-4F58-9827-09010DD3CF52}">
   <dimension ref="B2:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1558,18 +1820,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="21" x14ac:dyDescent="0.3">
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
       <c r="L2" s="45"/>
     </row>
     <row r="5" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1597,7 +1859,7 @@
         <v>9</v>
       </c>
       <c r="C7" s="47" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D7" s="47"/>
       <c r="E7" s="47"/>
@@ -1605,7 +1867,7 @@
       <c r="G7" s="47"/>
       <c r="H7" s="47"/>
       <c r="I7" s="11" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="J7" s="12" t="s">
         <v>25</v>
@@ -1626,46 +1888,66 @@
       <c r="I8" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="J8" s="12"/>
+      <c r="J8" s="12" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="9" spans="2:12" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="47"/>
+      <c r="C9" s="47" t="s">
+        <v>29</v>
+      </c>
       <c r="D9" s="47"/>
       <c r="E9" s="47"/>
       <c r="F9" s="47"/>
       <c r="G9" s="47"/>
       <c r="H9" s="47"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="12"/>
+      <c r="I9" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="10" spans="2:12" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="47"/>
+      <c r="C10" s="47" t="s">
+        <v>32</v>
+      </c>
       <c r="D10" s="47"/>
       <c r="E10" s="47"/>
       <c r="F10" s="47"/>
       <c r="G10" s="47"/>
       <c r="H10" s="47"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="12"/>
+      <c r="I10" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="11" spans="2:12" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="44"/>
+      <c r="C11" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="D11" s="44"/>
       <c r="E11" s="44"/>
       <c r="F11" s="44"/>
       <c r="G11" s="44"/>
       <c r="H11" s="44"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="14"/>
+      <c r="I11" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="J11" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1678,15 +1960,16 @@
     <mergeCell ref="C10:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA7DFC68-58FB-4A57-97A3-D7ABCCFA9375}">
-  <dimension ref="B2:J6"/>
+  <dimension ref="B2:J16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1695,16 +1978,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="21" x14ac:dyDescent="0.3">
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
       <c r="J2" s="45"/>
     </row>
     <row r="4" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1728,21 +2011,124 @@
       <c r="B6" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="44"/>
+      <c r="C6" s="44" t="s">
+        <v>45</v>
+      </c>
       <c r="D6" s="44"/>
       <c r="E6" s="44"/>
       <c r="F6" s="44"/>
       <c r="G6" s="44"/>
       <c r="H6" s="44"/>
-      <c r="I6" s="14"/>
+      <c r="I6" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B11" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="48"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="48"/>
+      <c r="H11" s="48"/>
+      <c r="I11" s="48"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B12" s="48"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="48"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B13" s="48"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="48"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="48"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B14" s="48"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="48"/>
+      <c r="H14" s="48"/>
+      <c r="I14" s="48"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B15" s="48"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="48"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B16" s="48"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="48"/>
+      <c r="H16" s="48"/>
+      <c r="I16" s="48"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
+    <mergeCell ref="B11:I16"/>
     <mergeCell ref="B2:J2"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="C6:H6"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="C8:H8"/>
   </mergeCells>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>